<commit_message>
Fixing link to catch unit CL in form
</commit_message>
<xml_diff>
--- a/forms/Form-3CE-multiple.xlsx
+++ b/forms/Form-3CE-multiple.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCF2B49-E4FF-4D64-9C92-056AD7360C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FD7580-C8EE-40F2-90C9-FF9E994B737F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="D/L7RJXD1bM7VSukp9nBPXamnS2mKwuV7VHnNS9bopG+/gy69KSPIxEDp2efAHIwM2oGVTU5uyDQpmk0iVlvLw==" workbookSaltValue="ZXtEfnD7/zBb2FnSisyo4w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -12319,7 +12319,7 @@
       <c r="DO1048576" s="84"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jacvmIeSZ3WaAsz8fQWUn/9o9RpqkLvrtOs36Evfq/04Dd+U4rYqkgXXYvXvhHsfbb90e2D/OQHC0x5FcwwIhQ==" saltValue="Xm7jQKQO7FTSUuQ4zB25JQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="T3:DO3"/>
     <mergeCell ref="B4:F4"/>
@@ -12355,9 +12355,9 @@
     <hyperlink ref="O5" r:id="rId9" location="effortUnits" xr:uid="{BBFE535B-6BD4-4ED0-A364-BCA2CB5FA9F2}"/>
     <hyperlink ref="Q5" r:id="rId10" location="effortUnits" xr:uid="{8E49C3AE-4385-4293-9432-CCAE0BAA4D5D}"/>
     <hyperlink ref="S4" r:id="rId11" location="species" xr:uid="{8B9FF7CF-5003-45EA-B86B-8B8135E02938}"/>
-    <hyperlink ref="S5" r:id="rId12" location="effortUnits" xr:uid="{E17AC96F-B121-450F-ADD7-91CBC2C50DA4}"/>
-    <hyperlink ref="J5" r:id="rId13" location="raisings" display="Data raising" xr:uid="{731DC286-6E5E-4BEF-A720-A65ED9B7C74D}"/>
-    <hyperlink ref="D5" r:id="rId14" location="species" xr:uid="{EA9ACA5D-6BBC-4111-B6DC-3673239327C3}"/>
+    <hyperlink ref="J5" r:id="rId12" location="raisings" display="Data raising" xr:uid="{731DC286-6E5E-4BEF-A720-A65ED9B7C74D}"/>
+    <hyperlink ref="D5" r:id="rId13" location="species" xr:uid="{EA9ACA5D-6BBC-4111-B6DC-3673239327C3}"/>
+    <hyperlink ref="S5" r:id="rId14" location="catchUnits" xr:uid="{E17AC96F-B121-450F-ADD7-91CBC2C50DA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>

</xml_diff>